<commit_message>
Soluzioni Excel 4 - Fine
</commit_message>
<xml_diff>
--- a/Soluzioni_Verifica.xlsx
+++ b/Soluzioni_Verifica.xlsx
@@ -1,133 +1,171 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC_HOME\Desktop\Pr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WS\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33442D5C-E0DB-4F8D-B55F-85A6805D574A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Versione A - Es.1" sheetId="3" r:id="rId1"/>
     <sheet name="Versione B - Es.1" sheetId="1" r:id="rId2"/>
     <sheet name="Versione A - Es.2" sheetId="4" r:id="rId3"/>
+    <sheet name="Versione B - Es.2" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'Versione A - Es.1'!$F$3:$F$5</definedName>
     <definedName name="solver_adj" localSheetId="2" hidden="1">'Versione A - Es.2'!$G$8:$G$9</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">'Versione B - Es.1'!$F$3:$F$5</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">'Versione B - Es.2'!$G$8:$G$9</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_drv" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Versione A - Es.1'!$F$3:$F$5</definedName>
     <definedName name="solver_lhs1" localSheetId="2" hidden="1">'Versione A - Es.2'!$G$8:$G$9</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Versione B - Es.1'!$F$3:$F$5</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">'Versione B - Es.2'!$G$9</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Versione A - Es.1'!$O$3:$S$3</definedName>
     <definedName name="solver_lhs2" localSheetId="2" hidden="1">'Versione A - Es.2'!$G$9</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Versione B - Es.1'!$O$3:$S$3</definedName>
+    <definedName name="solver_lhs2" localSheetId="3" hidden="1">'Versione B - Es.2'!$G$9</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Versione A - Es.1'!$O$3:$S$3</definedName>
     <definedName name="solver_lhs3" localSheetId="2" hidden="1">'Versione A - Es.2'!$G$9</definedName>
     <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Versione B - Es.1'!$O$3:$S$3</definedName>
+    <definedName name="solver_lhs3" localSheetId="3" hidden="1">'Versione B - Es.2'!$G$9</definedName>
     <definedName name="solver_lhs4" localSheetId="2" hidden="1">'Versione A - Es.2'!$G$9</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">4</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'Versione A - Es.1'!$F$8</definedName>
     <definedName name="solver_opt" localSheetId="2" hidden="1">'Versione A - Es.2'!$F$12</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">'Versione B - Es.1'!$F$8</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">'Versione B - Es.2'!$F$12</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">'Versione B - Es.2'!$K$10</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">'Versione A - Es.1'!$O$4:$S$4</definedName>
     <definedName name="solver_rhs2" localSheetId="2" hidden="1">'Versione A - Es.2'!$K$8</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">'Versione B - Es.1'!$O$4:$S$4</definedName>
+    <definedName name="solver_rhs2" localSheetId="3" hidden="1">'Versione B - Es.2'!$K$8</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs3" localSheetId="2" hidden="1">'Versione A - Es.2'!$K$10</definedName>
     <definedName name="solver_rhs3" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rhs3" localSheetId="3" hidden="1">'Versione B - Es.2'!$K$9</definedName>
     <definedName name="solver_rhs4" localSheetId="2" hidden="1">'Versione A - Es.2'!$K$9</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -148,7 +186,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
   <si>
     <t>X</t>
   </si>
@@ -222,7 +260,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -700,16 +738,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D2:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:19" x14ac:dyDescent="0.3">
       <c r="I2" s="5" t="s">
         <v>3</v>
       </c>
@@ -741,7 +779,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
@@ -790,7 +828,7 @@
         <v>115.00000000000001</v>
       </c>
     </row>
-    <row r="4" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
@@ -834,7 +872,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
@@ -863,7 +901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="4:19" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:19" ht="19.8" x14ac:dyDescent="0.4">
       <c r="E8" s="9" t="s">
         <v>8</v>
       </c>
@@ -878,16 +916,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="D2:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:19" x14ac:dyDescent="0.3">
       <c r="I2" s="5" t="s">
         <v>3</v>
       </c>
@@ -919,7 +957,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
@@ -968,7 +1006,7 @@
         <v>117.99999999999984</v>
       </c>
     </row>
-    <row r="4" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1012,7 +1050,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="4:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:19" x14ac:dyDescent="0.3">
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1041,7 +1079,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="4:19" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:19" ht="19.8" x14ac:dyDescent="0.4">
       <c r="E8" s="9" t="s">
         <v>8</v>
       </c>
@@ -1056,23 +1094,125 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="E3:K12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="5:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F3" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="5:11" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="F4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="5:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="F5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="14">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="8" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>4.3100051259654819</v>
+      </c>
+      <c r="H8" s="2">
+        <v>4</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="4">
+        <f>3+2/5*SIN(2*PI()/3*G8)</f>
+        <v>3.1550022757976457</v>
+      </c>
+    </row>
+    <row r="9" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>3.1550025629827783</v>
+      </c>
+      <c r="H9" s="2">
+        <v>5</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="4">
+        <f>2+2/5*SIN(2*PI()/3*G8)</f>
+        <v>2.1550022757976457</v>
+      </c>
+    </row>
+    <row r="10" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="J10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="4">
+        <f>1/2*G8+1</f>
+        <v>3.155002562982741</v>
+      </c>
+    </row>
+    <row r="11" spans="5:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="5:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="E12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="12">
+        <f>SUMPRODUCT(G8:G9,H8:H9)</f>
+        <v>33.015033318775821</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F3:H3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="E3:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="5:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="5:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F3" s="15" t="s">
         <v>22</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
     </row>
-    <row r="4" spans="5:11" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="5:11" ht="19.8" x14ac:dyDescent="0.4">
       <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
@@ -1080,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="5:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="5:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F5" s="3" t="s">
         <v>21</v>
       </c>
@@ -1088,7 +1228,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1096,20 +1236,20 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>4.3100051259654819</v>
+        <v>4.0582245251409175</v>
       </c>
       <c r="H8" s="2">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J8" s="10" t="s">
         <v>17</v>
       </c>
       <c r="K8" s="4">
-        <f>3+2/5*SIN(2*PI()/3*G8)</f>
-        <v>3.1550022757976457</v>
-      </c>
-    </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.25">
+        <f>3+1/7*POWER(G8,2)</f>
+        <v>5.3527408994936039</v>
+      </c>
+    </row>
+    <row r="9" spans="5:11" x14ac:dyDescent="0.3">
       <c r="E9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1117,7 +1257,7 @@
         <v>1</v>
       </c>
       <c r="G9">
-        <v>3.1550025629827783</v>
+        <v>4.3527415083802516</v>
       </c>
       <c r="H9" s="2">
         <v>5</v>
@@ -1126,27 +1266,27 @@
         <v>18</v>
       </c>
       <c r="K9" s="4">
-        <f>2+2/5*SIN(2*PI()/3*G8)</f>
-        <v>2.1550022757976457</v>
-      </c>
-    </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.25">
+        <f>2+1/7*POWER(G8,2)</f>
+        <v>4.3527408994936039</v>
+      </c>
+    </row>
+    <row r="10" spans="5:11" x14ac:dyDescent="0.3">
       <c r="J10" s="10" t="s">
         <v>19</v>
       </c>
       <c r="K10" s="4">
-        <f>1/2*G8+1</f>
-        <v>3.155002562982741</v>
-      </c>
-    </row>
-    <row r="11" spans="5:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="5:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+        <f>1/3*G8+3</f>
+        <v>4.3527415083803058</v>
+      </c>
+    </row>
+    <row r="11" spans="5:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="5:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E12" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="12">
         <f>SUMPRODUCT(G8:G9,H8:H9)</f>
-        <v>33.015033318775821</v>
+        <v>86.695299944155934</v>
       </c>
     </row>
   </sheetData>

</xml_diff>